<commit_message>
Last changes before completion of course
</commit_message>
<xml_diff>
--- a/05_Evaluation/recommendation_strategy_development_sheet.xlsx
+++ b/05_Evaluation/recommendation_strategy_development_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdanc\Desktop\HR_201_Employee_Attrition_Project\06_Deployment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidespinola/Desktop/DS4B_201_R_Employee_Attrition_Project/05_Evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8BFAADD7-5517-414A-B370-CD3FB25C09FC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA08B9E2-3B45-774B-B785-15DF0D76F987}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="520" windowWidth="35840" windowHeight="20380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Strategy Worksheet" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t>Feature</t>
   </si>
@@ -141,6 +141,123 @@
   </si>
   <si>
     <t xml:space="preserve"> Used to investigate the relationship between values within features and the target (Attrition = Yes)</t>
+  </si>
+  <si>
+    <t>Employees with high OT  are leaving</t>
+  </si>
+  <si>
+    <t>Reduce Overtime</t>
+  </si>
+  <si>
+    <t>Employees with Job Level 1 are leaving/ Job Level 2 are staying</t>
+  </si>
+  <si>
+    <t>Promote faster for high performers</t>
+  </si>
+  <si>
+    <t>Skip - Include in Executive Report</t>
+  </si>
+  <si>
+    <t>Zero Stock Option - Likely to leave</t>
+  </si>
+  <si>
+    <t>Single - More likely to leave</t>
+  </si>
+  <si>
+    <t>Low income - Bin1 is more  likely to leave</t>
+  </si>
+  <si>
+    <t>YAC- High -Likely to stay / YAC- Low-Likely to leave</t>
+  </si>
+  <si>
+    <t>TWY- High -Likely to stay / TWY- Low-Likely to leave</t>
+  </si>
+  <si>
+    <t>Tie low TWY to training and formation/mentorship activities</t>
+  </si>
+  <si>
+    <t>Skip- Covered by TWY</t>
+  </si>
+  <si>
+    <t>See - TWY</t>
+  </si>
+  <si>
+    <t>More time in current role is related to lower attrition</t>
+  </si>
+  <si>
+    <t>Incentivize specialization or promote</t>
+  </si>
+  <si>
+    <t>Certain JobRoles have higher attrition and need to be monitored more closely</t>
+  </si>
+  <si>
+    <t>See - YICR</t>
+  </si>
+  <si>
+    <t>Skip -Covered by YICR</t>
+  </si>
+  <si>
+    <t>Employees with low environment satisfaction are more likely to leave</t>
+  </si>
+  <si>
+    <t>Improve the workplace environment</t>
+  </si>
+  <si>
+    <t>Bad worklife balance is more likely to leave</t>
+  </si>
+  <si>
+    <t>Improve the worklife balance</t>
+  </si>
+  <si>
+    <t>More business travel - more likely to leave/Less business travel is more likely to stay</t>
+  </si>
+  <si>
+    <t>Reduce business travel where possible</t>
+  </si>
+  <si>
+    <t>High job involvement likely to stay/low job involvement likely to leave</t>
+  </si>
+  <si>
+    <t>Create personal development plan</t>
+  </si>
+  <si>
+    <t>Bin 4(High) more likely to leave</t>
+  </si>
+  <si>
+    <t>Low JS more likely to leave/ High JS more likely to stay</t>
+  </si>
+  <si>
+    <t>Low: Create a personal development plan/High: mentorship roles</t>
+  </si>
+  <si>
+    <t>Sales -More likely to leave/R&amp;D more likely to stay</t>
+  </si>
+  <si>
+    <t>Technical Degree - More education</t>
+  </si>
+  <si>
+    <t>Bin1 more likely to leave</t>
+  </si>
+  <si>
+    <t>High distance from Home - more likely to leave</t>
+  </si>
+  <si>
+    <t>monitor worklife balance</t>
+  </si>
+  <si>
+    <t>Work Life</t>
+  </si>
+  <si>
+    <t>Professional Development</t>
+  </si>
+  <si>
+    <t>Professional Development/Personal Development</t>
+  </si>
+  <si>
+    <t>Tie promotion if  low advance faster/Mentor if YAC low</t>
+  </si>
+  <si>
+    <t>Personal Development</t>
   </si>
 </sst>
 </file>
@@ -309,7 +426,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B6:E27" totalsRowShown="0">
-  <autoFilter ref="B6:E27" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <autoFilter ref="B6:E27" xr:uid="{00000000-0009-0000-0100-000001000000}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Work Life"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Feature"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Discussion (Hypothesis)"/>
@@ -587,26 +710,26 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <selection pane="bottomLeft" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" customWidth="1"/>
-    <col min="3" max="3" width="84.140625" customWidth="1"/>
-    <col min="4" max="4" width="57.7109375" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1"/>
-    <col min="6" max="7" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
+    <col min="3" max="3" width="84.1640625" customWidth="1"/>
+    <col min="4" max="4" width="57.6640625" customWidth="1"/>
+    <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="6" max="7" width="36.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:5" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="2:5" s="2" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:5" s="2" customFormat="1" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -615,7 +738,7 @@
       </c>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
@@ -624,8 +747,8 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="2:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" ht="4.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>0</v>
       </c>
@@ -639,112 +762,271 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>51</v>
+      </c>
+      <c r="E18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>65</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>30</v>
       </c>
@@ -752,7 +1034,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="2:3" ht="3.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:5" ht="3.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>